<commit_message>
Se actualiza texto en about y otros cambios menores
</commit_message>
<xml_diff>
--- a/Casos_de_tests.xlsx
+++ b/Casos_de_tests.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>Nombre del Proyecto</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Una vez que se carga el comentario en el detalle del instrumento, el usuario es dirigido al inicio</t>
   </si>
   <si>
-    <t>Edición de Perfil de Usuario</t>
-  </si>
-  <si>
     <t>Logout</t>
   </si>
   <si>
@@ -116,13 +113,37 @@
   </si>
   <si>
     <t>Que no se puedan visualizar y redirija al login</t>
+  </si>
+  <si>
+    <t>los cambios se realizan y persisten sin problemas</t>
+  </si>
+  <si>
+    <t>Poder eliminar el registro seleccionado</t>
+  </si>
+  <si>
+    <t>El registro se elimina sin problemas</t>
+  </si>
+  <si>
+    <t>Buscar con cualquier dato de un Host</t>
+  </si>
+  <si>
+    <t>Encontrar un registro mediante el ingreso de un valor de referencia</t>
+  </si>
+  <si>
+    <t>Devuelve correctamente resultados si hay coincidencia</t>
+  </si>
+  <si>
+    <t>Editar los campos correspondientes en contactos</t>
+  </si>
+  <si>
+    <t>cambiar cualquiera de los campos correspondiente a un contacto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,14 +153,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -214,15 +227,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,7 +544,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,68 +558,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8">
         <v>1</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="10">
-        <v>1</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="8"/>
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="10"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -676,13 +689,13 @@
         <v>45493</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="E9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>17</v>
@@ -696,13 +709,13 @@
         <v>45493</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="E10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>17</v>
@@ -716,7 +729,7 @@
         <v>45493</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>19</v>
@@ -728,7 +741,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>6</v>
       </c>
@@ -736,15 +749,19 @@
         <v>45493</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="F12" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>7</v>
       </c>
@@ -752,15 +769,19 @@
         <v>45493</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="F13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>8</v>
       </c>
@@ -768,10 +789,14 @@
         <v>45493</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="F14" s="2" t="s">
         <v>17</v>
       </c>
@@ -784,7 +809,7 @@
         <v>45493</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -800,13 +825,13 @@
         <v>45493</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>33</v>
+      <c r="E16" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>17</v>

</xml_diff>